<commit_message>
update salt marsh materials
</commit_message>
<xml_diff>
--- a/saltmarsh/final_spreadsheets/marsh_composition_and_allometry_data_entry_spreadsheet_marinegeo.xlsx
+++ b/saltmarsh/final_spreadsheets/marsh_composition_and_allometry_data_entry_spreadsheet_marinegeo.xlsx
@@ -118,6 +118,18 @@
     <t xml:space="preserve">non-living cover data</t>
   </si>
   <si>
+    <t xml:space="preserve">bush_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An numeric identifier for each shrub measured in the quadrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shrub dimensions and stem count, shrub stem measurements</t>
+  </si>
+  <si>
     <t xml:space="preserve">cover_code</t>
   </si>
   <si>
@@ -148,9 +160,6 @@
     <t xml:space="preserve">The x dimension of the shrub in centimeters</t>
   </si>
   <si>
-    <t xml:space="preserve">numeric</t>
-  </si>
-  <si>
     <t xml:space="preserve">centimeters</t>
   </si>
   <si>
@@ -293,15 +302,6 @@
   </si>
   <si>
     <t xml:space="preserve">shrub_dimensions_notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shrub_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional; use a numeric identifier for each shrub measured in the quadrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shrub dimensions and stem count, shrub stem measurements</t>
   </si>
   <si>
     <t xml:space="preserve">shrub_stem_measurements_notes</t>
@@ -1087,20 +1087,20 @@
         <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>13</v>
@@ -1108,15 +1108,15 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>13</v>
@@ -1124,79 +1124,77 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="C12" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="10" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
@@ -1204,47 +1202,49 @@
         <v>44</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
@@ -1252,7 +1252,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>13</v>
@@ -1260,18 +1260,18 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1297,17 +1297,15 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
         <v>23</v>
@@ -1315,54 +1313,54 @@
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="25">
@@ -1373,14 +1371,14 @@
         <v>66</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>67</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
@@ -1391,14 +1389,14 @@
         <v>69</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27">
@@ -1409,14 +1407,14 @@
         <v>72</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28">
@@ -1427,20 +1425,22 @@
         <v>75</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>13</v>
@@ -1448,23 +1448,23 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
@@ -1472,20 +1472,20 @@
         <v>81</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>17</v>
@@ -1496,23 +1496,23 @@
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
@@ -1557,7 +1557,7 @@
         <v>91</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -1573,7 +1573,7 @@
         <v>93</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -1589,12 +1589,12 @@
         <v>95</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39">
@@ -1605,12 +1605,12 @@
         <v>97</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40">
@@ -1621,7 +1621,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10" t="s">
@@ -1639,7 +1639,7 @@
         <v>102</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10" t="s">
@@ -1657,7 +1657,7 @@
         <v>104</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10" t="s">
@@ -1675,11 +1675,11 @@
         <v>106</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>20</v>
@@ -1693,7 +1693,7 @@
         <v>108</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -1709,7 +1709,7 @@
         <v>110</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -1725,12 +1725,12 @@
         <v>112</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47">
@@ -1741,7 +1741,7 @@
         <v>114</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -1802,25 +1802,25 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1855,34 +1855,34 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1921,46 +1921,46 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>90</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>113</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1997,37 +1997,37 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>92</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>16</v>
@@ -2068,28 +2068,28 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>107</v>
@@ -2139,34 +2139,34 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2192,7 @@
     <col min="7" max="7" width="7.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="20.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="12.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="7.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="16.71" hidden="0" customWidth="1"/>
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="9.71" hidden="0" customWidth="1"/>
@@ -2206,31 +2206,31 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>94</v>
@@ -2239,16 +2239,16 @@
         <v>96</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2274,7 +2274,7 @@
     <col min="7" max="7" width="7.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="20.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="12.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="7.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="11.71" hidden="0" customWidth="1"/>
     <col min="12" max="12" width="16.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="13.71" hidden="0" customWidth="1"/>
@@ -2286,31 +2286,31 @@
         <v>87</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>107</v>

</xml_diff>